<commit_message>
updated BOM for 5 boards
</commit_message>
<xml_diff>
--- a/3. Design/BOM.xlsx
+++ b/3. Design/BOM.xlsx
@@ -7,11 +7,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="estimativa 20 inversores" sheetId="3" r:id="rId3"/>
-    <sheet name="racio_custo" sheetId="4" r:id="rId4"/>
-    <sheet name="lojas" sheetId="5" r:id="rId5"/>
+    <sheet name="BOM" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="estimativa 20 inversores" sheetId="3" r:id="rId4"/>
+    <sheet name="racio_custo" sheetId="4" r:id="rId5"/>
+    <sheet name="lojas" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="306">
   <si>
     <t>Comment</t>
   </si>
@@ -821,12 +822,135 @@
   </si>
   <si>
     <t>R2, R3, R4</t>
+  </si>
+  <si>
+    <t>Bloque de terminal PCB, paso5mm 2 Contacto Macho Recta Bloque de terminales PCB, montaje: Montaje en PCB</t>
+  </si>
+  <si>
+    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 1206 50V 10uF 20% X5R</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>price total</t>
+  </si>
+  <si>
+    <t>Condensadores de tântalo - revestimento sólido de SMD 50V 10uF 10% ESR=0.8Ohms</t>
+  </si>
+  <si>
+    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 10nF 50V X7R 10%</t>
+  </si>
+  <si>
+    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 10uF 25V X5R +/-10% 0805 Gen Purp</t>
+  </si>
+  <si>
+    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 0805 50V 1uF 20% X5R</t>
+  </si>
+  <si>
+    <t>Sensores de Corrente de Montagem de Painel Hall Effect IC LF 30A 66 mV/A</t>
+  </si>
+  <si>
+    <t>Capacitores eletrolíticos de alumínio - terminal de pressão 450V 470uF 20% Tol.</t>
+  </si>
+  <si>
+    <t>512-1N4148TR</t>
+  </si>
+  <si>
+    <t>Diodos - Fins gerais, energia, comutação Hi Conductance Fast</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 1/8Watt 100ohms 1% Commercial Use</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 3.6K 5%</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 1/8Watt 1Kohms 1% Commercial Use</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 0805 1K8ohm 5% Anti Surge AEC-Q200</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 0805 3Kohms 5% Tol AEC-Q200</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 1/8Watt 0ohms Commercial Use</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 0805 30Kohms 1% AEC-Q200</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 1/8Watt 330ohms 1% Commercial Use</t>
+  </si>
+  <si>
+    <t>71-CRCW0805-150-E3</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 1/8watt 150ohms 1% 100ppm</t>
+  </si>
+  <si>
+    <t>Controladores e drivers de Motor/Movimento/Ignição IFPS MODULES</t>
+  </si>
+  <si>
+    <t>Conversores CC/CC com isolação 1W 5Vin 5Vout 200mA SIP7</t>
+  </si>
+  <si>
+    <t>Amplificadores de isolamento 4kV peak Iso Amp</t>
+  </si>
+  <si>
+    <t>LEDs padrão - SMD GREEN WATER CLEAR</t>
+  </si>
+  <si>
+    <t>71-CRCW08055K60FKEA</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 1/8watt 5.6Kohms 1%</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 0805 7.5Kohms 1% AEC-Q200</t>
+  </si>
+  <si>
+    <t>Portas lógicas QUADRUPLE 2-INPUT NAND GATE</t>
+  </si>
+  <si>
+    <t>Header 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9751343 (farnell)</t>
+  </si>
+  <si>
+    <t>B32653A6474K000 -  DC Film Capacitor, 0.47 µF, 630 V, Metallized PP, ± 10%, B32653 Series</t>
+  </si>
+  <si>
+    <t>MCLRP12FTWRR039 -  SMD Current Sense Resistor, 0.039 ohm, LRP Series, 2512 [6432 Metric], 3 W, ± 1%, Metal Strip</t>
+  </si>
+  <si>
+    <t>3 Position Header Spacer Connector 0.100" (2.54mm) Gold Through Hole</t>
+  </si>
+  <si>
+    <t>HW-03-14-G-S-1218-055-ND (digikey)</t>
+  </si>
+  <si>
+    <t>ver alternativas</t>
+  </si>
+  <si>
+    <t>Connector Header position</t>
+  </si>
+  <si>
+    <t>TMM-124-03-G-S-ND (digikey)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -883,7 +1007,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -911,6 +1035,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -989,7 +1119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1033,6 +1163,28 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1314,9 +1466,1353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.85546875" style="30" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3">
+        <f t="shared" ref="I2:I30" si="0">H2+G2</f>
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="L2" s="29">
+        <v>50</v>
+      </c>
+      <c r="M2" s="32">
+        <v>0.24</v>
+      </c>
+      <c r="N2" s="32">
+        <f>L2*M2</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="L3" s="29">
+        <v>30</v>
+      </c>
+      <c r="M3" s="32">
+        <v>0.31</v>
+      </c>
+      <c r="N3" s="32">
+        <f t="shared" ref="N3:N30" si="1">L3*M3</f>
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="3">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="L4" s="29">
+        <v>50</v>
+      </c>
+      <c r="M4" s="32">
+        <v>1.58</v>
+      </c>
+      <c r="N4" s="32">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="L5" s="29">
+        <v>50</v>
+      </c>
+      <c r="M5" s="32">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="N5" s="32">
+        <f t="shared" si="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="L6" s="29">
+        <v>60</v>
+      </c>
+      <c r="M6" s="32">
+        <v>0.108</v>
+      </c>
+      <c r="N6" s="32">
+        <f t="shared" si="1"/>
+        <v>6.4799999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="L7" s="29">
+        <v>50</v>
+      </c>
+      <c r="M7" s="32">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N7" s="32">
+        <f>L7*M7</f>
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="L8" s="29">
+        <v>20</v>
+      </c>
+      <c r="M8" s="32">
+        <v>2.77</v>
+      </c>
+      <c r="N8" s="32">
+        <f t="shared" si="1"/>
+        <v>55.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="L9" s="29">
+        <v>20</v>
+      </c>
+      <c r="M9" s="32">
+        <v>5.58</v>
+      </c>
+      <c r="N9" s="32">
+        <f t="shared" si="1"/>
+        <v>111.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="L10" s="29">
+        <v>5</v>
+      </c>
+      <c r="M10" s="32">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="N10" s="32">
+        <f t="shared" si="1"/>
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="L11" s="29">
+        <v>20</v>
+      </c>
+      <c r="M11" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="N11" s="32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="3">
+        <v>8</v>
+      </c>
+      <c r="H12" s="3">
+        <v>8</v>
+      </c>
+      <c r="I12" s="3">
+        <v>16</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="L12" s="29">
+        <v>1</v>
+      </c>
+      <c r="M12" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="N12" s="32">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="O12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="3">
+        <v>8</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="L13" s="29">
+        <v>1</v>
+      </c>
+      <c r="M13" s="32">
+        <v>3.55</v>
+      </c>
+      <c r="N13" s="32">
+        <f t="shared" si="1"/>
+        <v>3.55</v>
+      </c>
+      <c r="O13" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="3">
+        <v>9</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="L14" s="29">
+        <v>50</v>
+      </c>
+      <c r="M14" s="32">
+        <v>4.7E-2</v>
+      </c>
+      <c r="N14" s="32">
+        <f t="shared" si="1"/>
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="L15" s="29">
+        <v>20</v>
+      </c>
+      <c r="M15" s="32">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="N15" s="32">
+        <f t="shared" si="1"/>
+        <v>5.1400000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="L16" s="29">
+        <v>10</v>
+      </c>
+      <c r="M16" s="32">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="N16" s="32">
+        <f t="shared" si="1"/>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="L17" s="29">
+        <v>10</v>
+      </c>
+      <c r="M17" s="32">
+        <v>5.5E-2</v>
+      </c>
+      <c r="N17" s="32">
+        <f t="shared" si="1"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="L18" s="29">
+        <v>10</v>
+      </c>
+      <c r="M18" s="32">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="N18" s="32">
+        <f t="shared" si="1"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K19" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="L19" s="29">
+        <v>10</v>
+      </c>
+      <c r="M19" s="32">
+        <v>5.5E-2</v>
+      </c>
+      <c r="N19" s="32">
+        <f t="shared" si="1"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="L20" s="29">
+        <v>10</v>
+      </c>
+      <c r="M20" s="32">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N20" s="32">
+        <f t="shared" si="1"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="54" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="3">
+        <v>8</v>
+      </c>
+      <c r="H21" s="3">
+        <v>30</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="L21" s="29">
+        <v>200</v>
+      </c>
+      <c r="M21" s="32">
+        <v>0.02</v>
+      </c>
+      <c r="N21" s="32">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K22" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="L22" s="29">
+        <v>30</v>
+      </c>
+      <c r="M22" s="32">
+        <v>4.7E-2</v>
+      </c>
+      <c r="N22" s="32">
+        <f t="shared" si="1"/>
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>3</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="L23" s="29">
+        <v>30</v>
+      </c>
+      <c r="M23" s="32">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="N23" s="32">
+        <f t="shared" si="1"/>
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K24" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="L24" s="29">
+        <v>6</v>
+      </c>
+      <c r="M24" s="32">
+        <v>16.25</v>
+      </c>
+      <c r="N24" s="32">
+        <f t="shared" si="1"/>
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>3</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="L25" s="29">
+        <v>25</v>
+      </c>
+      <c r="M25" s="32">
+        <v>1.31</v>
+      </c>
+      <c r="N25" s="32">
+        <f t="shared" si="1"/>
+        <v>32.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K26" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="L26" s="29">
+        <v>20</v>
+      </c>
+      <c r="M26" s="32">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="N26" s="32">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="3">
+        <v>2</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="L27" s="29">
+        <v>10</v>
+      </c>
+      <c r="M27" s="32">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="N27" s="32">
+        <f t="shared" si="1"/>
+        <v>2.8100000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="3">
+        <v>8</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="L28" s="29">
+        <v>50</v>
+      </c>
+      <c r="M28" s="32">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="N28" s="32">
+        <f t="shared" si="1"/>
+        <v>2.9499999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="3">
+        <v>8</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="K29" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="L29" s="29">
+        <v>50</v>
+      </c>
+      <c r="M29" s="32">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="N29" s="32">
+        <f t="shared" si="1"/>
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="3">
+        <v>3</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="K30" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="L30" s="29">
+        <v>20</v>
+      </c>
+      <c r="M30" s="32">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="N30" s="32">
+        <f t="shared" si="1"/>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>305</v>
+      </c>
+      <c r="N31" s="34">
+        <f>SUM(N2:N30)</f>
+        <v>541.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2685,7 +4181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
@@ -3461,7 +4957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S35"/>
   <sheetViews>
@@ -5345,7 +6841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
@@ -6648,7 +8144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D10"/>
   <sheetViews>

</xml_diff>

<commit_message>
added 3ph psim simulation, 1ph psim simulation and updated XMC code
</commit_message>
<xml_diff>
--- a/3. Design/BOM.xlsx
+++ b/3. Design/BOM.xlsx
@@ -7,12 +7,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM" sheetId="6" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="estimativa 20 inversores" sheetId="3" r:id="rId4"/>
-    <sheet name="racio_custo" sheetId="4" r:id="rId5"/>
-    <sheet name="lojas" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="8" r:id="rId1"/>
+    <sheet name="BOM (3inv)" sheetId="7" r:id="rId2"/>
+    <sheet name="BOM" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="estimativa 20 inversores" sheetId="3" r:id="rId6"/>
+    <sheet name="racio_custo" sheetId="4" r:id="rId7"/>
+    <sheet name="lojas" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="357">
   <si>
     <t>Comment</t>
   </si>
@@ -942,16 +944,174 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>FALTA</t>
+  </si>
+  <si>
+    <t>relé de estado sólido</t>
+  </si>
+  <si>
+    <t>XMC4500</t>
+  </si>
+  <si>
+    <t>espaçadores</t>
+  </si>
+  <si>
+    <t>terminais molex</t>
+  </si>
+  <si>
+    <t>conectores xmc4500</t>
+  </si>
+  <si>
+    <t>espaçadores suporte dissipador</t>
+  </si>
+  <si>
+    <t>conectores phoenix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">538-105431-1103 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribuidores e Alojamento de Fios NANO-FIT HDR SMT VT SGL 3CKT TIN BLK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">538-145130-0300 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cabos de força DC Nano-Fit 75mm Cbl SR 3Ckt Blk </t>
+  </si>
+  <si>
+    <t>NÃO TESTADOS</t>
+  </si>
+  <si>
+    <t>MC34631 - Wire-To-Board Connector, Vertical, 2.54 mm, 3 Contacts, Header, MC34 Series, Through Hole, 1 Rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC34483 -  Connector Housing, MC34 Series, Receptacle, 3 Ways, 2.54 mm, 2218T Crimp Contacts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contacto de terminal de crimpado Molex 08-50-0032, KK, 4809, Hembra, Crimpado, Revestimiento de Estaño </t>
+  </si>
+  <si>
+    <t xml:space="preserve">558-MCX240D5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MCX240D5 </t>
+  </si>
+  <si>
+    <t>Relês - Montagem do PCB SIP SSR 280VAC/5A 3-15VDC In, ZC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+KIT_XMC45_RELAX_LITE_V1 -  Evaluation Board, XMC4500 MCU, Detachable On-Board Debugger, USB Powered </t>
+  </si>
+  <si>
+    <t>XMC male bars</t>
+  </si>
+  <si>
+    <t>251-8418</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cabezal de pines, RS PRO, Recta 72 pines 2 filas paso 2.54mm, Terminación Soldada, Orificio Pasante </t>
+  </si>
+  <si>
+    <t>XMC female bars</t>
+  </si>
+  <si>
+    <t>Conector hembra para PCB ASSMANN WSW Recta 40 pines 2 filas paso 2.54mm Montaje Orificio Pasante</t>
+  </si>
+  <si>
+    <t>674-2369</t>
+  </si>
+  <si>
+    <t>102-6570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEX. THREADED SPACER 8IO/10 </t>
+  </si>
+  <si>
+    <t>suporte dissipador</t>
+  </si>
+  <si>
+    <t>phoenix male</t>
+  </si>
+  <si>
+    <t>phoenix female</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+691313510002 -  Terminal Block, Header, 5.08 mm, 2 Ways, 20 A, 300 V, Through Hole Right Angle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1641993 </t>
+  </si>
+  <si>
+    <t>897-1159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloque de terminal PCB, paso5mm 2 Contacto Hembra Ángulo de 90° Macho, montaje: Montaje en PCB </t>
+  </si>
+  <si>
+    <t>espaçadores M3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+D01496 -  Standoff, Nylon 6.6 (Polyamide 6.6), M3, Hex Male-Female, 10 mm, 16 mm </t>
+  </si>
+  <si>
+    <t>fornecedor</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>FARNELL</t>
+  </si>
+  <si>
+    <t>VPN</t>
+  </si>
+  <si>
+    <t>896-6696</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9751343 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1675765 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1675755 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">467-598 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2828259 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2443552</t>
+  </si>
+  <si>
+    <t>1733428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KIT_XMC45_RELAX_LITE_V1 -  Evaluation Board, XMC4500 MCU, Detachable On-Board Debugger, USB Powered </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D01496 -  Standoff, Nylon 6.6 (Polyamide 6.6), M3, Hex Male-Female, 10 mm, 16 mm </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;€&quot;"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="170" formatCode="#,##0.000\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1006,6 +1166,20 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1045,7 +1219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1114,12 +1288,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1178,19 +1396,299 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="#,##0.000\ &quot;€&quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1201,6 +1699,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F41" totalsRowShown="0" tableBorderDxfId="6">
+  <autoFilter ref="A1:F41"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="fornecedor" dataDxfId="5"/>
+    <tableColumn id="2" name="VPN" dataDxfId="4"/>
+    <tableColumn id="3" name="Description" dataDxfId="3"/>
+    <tableColumn id="4" name="Quantity" dataDxfId="2"/>
+    <tableColumn id="5" name="price" dataDxfId="1"/>
+    <tableColumn id="6" name="price total" dataDxfId="0">
+      <calculatedColumnFormula>D2*E2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1466,10 +1981,2826 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" style="44" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" style="44" customWidth="1"/>
+    <col min="3" max="3" width="86.28515625" style="44" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="44" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="54" t="s">
+        <v>343</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>268</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="46">
+        <v>20</v>
+      </c>
+      <c r="E2" s="47">
+        <v>0.24</v>
+      </c>
+      <c r="F2" s="57">
+        <f>D2*E2</f>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" s="46">
+        <v>20</v>
+      </c>
+      <c r="E3" s="47">
+        <v>0.31</v>
+      </c>
+      <c r="F3" s="57">
+        <f t="shared" ref="F3:F41" si="0">D3*E3</f>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4" s="46">
+        <v>20</v>
+      </c>
+      <c r="E4" s="47">
+        <v>1.58</v>
+      </c>
+      <c r="F4" s="57">
+        <f t="shared" si="0"/>
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="46">
+        <v>50</v>
+      </c>
+      <c r="E5" s="47">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F5" s="57">
+        <f t="shared" si="0"/>
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>272</v>
+      </c>
+      <c r="D6" s="46">
+        <v>60</v>
+      </c>
+      <c r="E6" s="47">
+        <v>0.108</v>
+      </c>
+      <c r="F6" s="57">
+        <f t="shared" si="0"/>
+        <v>6.4799999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="D7" s="46">
+        <v>50</v>
+      </c>
+      <c r="E7" s="47">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F7" s="57">
+        <f>D7*E7</f>
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="D8" s="46">
+        <v>10</v>
+      </c>
+      <c r="E8" s="47">
+        <v>2.77</v>
+      </c>
+      <c r="F8" s="57">
+        <f t="shared" si="0"/>
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>275</v>
+      </c>
+      <c r="D9" s="46">
+        <v>20</v>
+      </c>
+      <c r="E9" s="47">
+        <v>5.58</v>
+      </c>
+      <c r="F9" s="57">
+        <f t="shared" si="0"/>
+        <v>111.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="55" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="D10" s="46">
+        <v>2</v>
+      </c>
+      <c r="E10" s="47">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F10" s="57">
+        <f t="shared" si="0"/>
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>277</v>
+      </c>
+      <c r="D11" s="46">
+        <v>20</v>
+      </c>
+      <c r="E11" s="47">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>314</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>315</v>
+      </c>
+      <c r="D12" s="46">
+        <v>20</v>
+      </c>
+      <c r="E12" s="47">
+        <v>1.49</v>
+      </c>
+      <c r="F12" s="57">
+        <f t="shared" si="0"/>
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>316</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>317</v>
+      </c>
+      <c r="D13" s="46">
+        <v>10</v>
+      </c>
+      <c r="E13" s="47">
+        <v>2.92</v>
+      </c>
+      <c r="F13" s="57">
+        <f t="shared" si="0"/>
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="55" t="s">
+        <v>345</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>349</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>319</v>
+      </c>
+      <c r="D14" s="46">
+        <v>50</v>
+      </c>
+      <c r="E14" s="47">
+        <v>2.9100000000000001E-2</v>
+      </c>
+      <c r="F14" s="57">
+        <f t="shared" si="0"/>
+        <v>1.4550000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="55" t="s">
+        <v>345</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>320</v>
+      </c>
+      <c r="D15" s="46">
+        <v>50</v>
+      </c>
+      <c r="E15" s="47">
+        <v>2.75E-2</v>
+      </c>
+      <c r="F15" s="57">
+        <f t="shared" si="0"/>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>351</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>321</v>
+      </c>
+      <c r="D16" s="46">
+        <v>200</v>
+      </c>
+      <c r="E16" s="47">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F16" s="57">
+        <f t="shared" si="0"/>
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>278</v>
+      </c>
+      <c r="D17" s="46">
+        <v>50</v>
+      </c>
+      <c r="E17" s="47">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F17" s="57">
+        <f t="shared" si="0"/>
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="55" t="s">
+        <v>345</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="D18" s="46">
+        <v>20</v>
+      </c>
+      <c r="E18" s="47">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="F18" s="57">
+        <f t="shared" si="0"/>
+        <v>5.1400000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>279</v>
+      </c>
+      <c r="D19" s="46">
+        <v>10</v>
+      </c>
+      <c r="E19" s="47">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F19" s="57">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>280</v>
+      </c>
+      <c r="D20" s="46">
+        <v>10</v>
+      </c>
+      <c r="E20" s="47">
+        <v>5.5E-2</v>
+      </c>
+      <c r="F20" s="57">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="D21" s="46">
+        <v>10</v>
+      </c>
+      <c r="E21" s="47">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="F21" s="57">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>282</v>
+      </c>
+      <c r="D22" s="46">
+        <v>10</v>
+      </c>
+      <c r="E22" s="47">
+        <v>5.5E-2</v>
+      </c>
+      <c r="F22" s="57">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>283</v>
+      </c>
+      <c r="D23" s="46">
+        <v>10</v>
+      </c>
+      <c r="E23" s="47">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="F23" s="57">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>284</v>
+      </c>
+      <c r="D24" s="46">
+        <v>200</v>
+      </c>
+      <c r="E24" s="47">
+        <v>0.02</v>
+      </c>
+      <c r="F24" s="57">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>285</v>
+      </c>
+      <c r="D25" s="46">
+        <v>30</v>
+      </c>
+      <c r="E25" s="47">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F25" s="57">
+        <f t="shared" si="0"/>
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>286</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>287</v>
+      </c>
+      <c r="D26" s="46">
+        <v>30</v>
+      </c>
+      <c r="E26" s="47">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F26" s="57">
+        <f t="shared" si="0"/>
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" s="46">
+        <v>4</v>
+      </c>
+      <c r="E27" s="47">
+        <v>16.25</v>
+      </c>
+      <c r="F27" s="57">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>289</v>
+      </c>
+      <c r="D28" s="46">
+        <v>15</v>
+      </c>
+      <c r="E28" s="47">
+        <v>1.37</v>
+      </c>
+      <c r="F28" s="57">
+        <f t="shared" si="0"/>
+        <v>20.55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="46">
+        <v>12</v>
+      </c>
+      <c r="E29" s="47">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F29" s="57">
+        <f t="shared" si="0"/>
+        <v>49.800000000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>291</v>
+      </c>
+      <c r="D30" s="46">
+        <v>10</v>
+      </c>
+      <c r="E30" s="47">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="F30" s="57">
+        <f t="shared" si="0"/>
+        <v>2.8100000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>292</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="D31" s="46">
+        <v>50</v>
+      </c>
+      <c r="E31" s="47">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F31" s="57">
+        <f t="shared" si="0"/>
+        <v>2.9499999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="C32" s="46" t="s">
+        <v>294</v>
+      </c>
+      <c r="D32" s="46">
+        <v>50</v>
+      </c>
+      <c r="E32" s="47">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F32" s="57">
+        <f t="shared" si="0"/>
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="45" t="s">
+        <v>218</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>295</v>
+      </c>
+      <c r="D33" s="46">
+        <v>10</v>
+      </c>
+      <c r="E33" s="47">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="F33" s="57">
+        <f t="shared" si="0"/>
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="45" t="s">
+        <v>322</v>
+      </c>
+      <c r="C34" s="46" t="s">
+        <v>324</v>
+      </c>
+      <c r="D34" s="46">
+        <v>2</v>
+      </c>
+      <c r="E34" s="47">
+        <v>16.079999999999998</v>
+      </c>
+      <c r="F34" s="57">
+        <f t="shared" si="0"/>
+        <v>32.159999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="55" t="s">
+        <v>345</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="D35" s="46">
+        <v>2</v>
+      </c>
+      <c r="E35" s="47">
+        <v>11.4</v>
+      </c>
+      <c r="F35" s="57">
+        <f t="shared" si="0"/>
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="B36" s="45" t="s">
+        <v>327</v>
+      </c>
+      <c r="C36" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="D36" s="46">
+        <v>10</v>
+      </c>
+      <c r="E36" s="47">
+        <v>3.2280000000000002</v>
+      </c>
+      <c r="F36" s="57">
+        <f t="shared" si="0"/>
+        <v>32.28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="B37" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="D37" s="46">
+        <v>5</v>
+      </c>
+      <c r="E37" s="47">
+        <v>1.6859999999999999</v>
+      </c>
+      <c r="F37" s="57">
+        <f t="shared" si="0"/>
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="B38" s="45" t="s">
+        <v>332</v>
+      </c>
+      <c r="C38" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="D38" s="46">
+        <v>20</v>
+      </c>
+      <c r="E38" s="47">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="F38" s="57">
+        <f t="shared" si="0"/>
+        <v>6.74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="55" t="s">
+        <v>345</v>
+      </c>
+      <c r="B39" s="50" t="s">
+        <v>338</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="D39" s="46">
+        <v>20</v>
+      </c>
+      <c r="E39" s="47">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F39" s="57">
+        <f t="shared" si="0"/>
+        <v>4.6999999999999993</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="B40" s="45" t="s">
+        <v>339</v>
+      </c>
+      <c r="C40" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="D40" s="46">
+        <v>20</v>
+      </c>
+      <c r="E40" s="47">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="F40" s="57">
+        <f t="shared" si="0"/>
+        <v>8.32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="58" t="s">
+        <v>345</v>
+      </c>
+      <c r="B41" s="59" t="s">
+        <v>354</v>
+      </c>
+      <c r="C41" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="D41" s="60">
+        <v>110</v>
+      </c>
+      <c r="E41" s="61">
+        <v>0.106</v>
+      </c>
+      <c r="F41" s="62">
+        <f t="shared" si="0"/>
+        <v>11.66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C42" s="51"/>
+      <c r="E42" s="52" t="s">
+        <v>305</v>
+      </c>
+      <c r="F42" s="53">
+        <f>SUM(F2:F41)</f>
+        <v>568.68000000000006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P53"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O42" sqref="J1:O42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.85546875" style="30" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3">
+        <f t="shared" ref="I2:I40" si="0">H2+G2</f>
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="M2" s="29">
+        <v>20</v>
+      </c>
+      <c r="N2" s="37">
+        <v>0.24</v>
+      </c>
+      <c r="O2" s="32">
+        <f>M2*N2</f>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="M3" s="29">
+        <v>20</v>
+      </c>
+      <c r="N3" s="37">
+        <v>0.31</v>
+      </c>
+      <c r="O3" s="32">
+        <f t="shared" ref="O3:O40" si="1">M3*N3</f>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="3">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="M4" s="29">
+        <v>20</v>
+      </c>
+      <c r="N4" s="37">
+        <v>1.58</v>
+      </c>
+      <c r="O4" s="32">
+        <f t="shared" si="1"/>
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L5" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="M5" s="29">
+        <v>50</v>
+      </c>
+      <c r="N5" s="37">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="O5" s="32">
+        <f t="shared" si="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L6" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="M6" s="29">
+        <v>60</v>
+      </c>
+      <c r="N6" s="37">
+        <v>0.108</v>
+      </c>
+      <c r="O6" s="32">
+        <f t="shared" si="1"/>
+        <v>6.4799999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="M7" s="29">
+        <v>50</v>
+      </c>
+      <c r="N7" s="37">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="O7" s="32">
+        <f>M7*N7</f>
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="M8" s="29">
+        <v>10</v>
+      </c>
+      <c r="N8" s="37">
+        <v>2.77</v>
+      </c>
+      <c r="O8" s="32">
+        <f t="shared" si="1"/>
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="M9" s="29">
+        <v>20</v>
+      </c>
+      <c r="N9" s="37">
+        <v>5.58</v>
+      </c>
+      <c r="O9" s="32">
+        <f t="shared" si="1"/>
+        <v>111.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="L10" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="M10" s="29">
+        <v>2</v>
+      </c>
+      <c r="N10" s="37">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="O10" s="32">
+        <f t="shared" si="1"/>
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="L11" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="M11" s="29">
+        <v>20</v>
+      </c>
+      <c r="N11" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="O11" s="32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="3">
+        <v>8</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3">
+        <v>16</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="L12" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="M12" s="29">
+        <v>20</v>
+      </c>
+      <c r="N12" s="37">
+        <v>1.49</v>
+      </c>
+      <c r="O12" s="32">
+        <f t="shared" ref="O12:O13" si="2">M12*N12</f>
+        <v>29.8</v>
+      </c>
+      <c r="P12" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="3">
+        <v>8</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3">
+        <f t="shared" ref="I13" si="3">H13+G13</f>
+        <v>8</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="L13" s="35" t="s">
+        <v>317</v>
+      </c>
+      <c r="M13" s="29">
+        <v>10</v>
+      </c>
+      <c r="N13" s="37">
+        <v>2.92</v>
+      </c>
+      <c r="O13" s="32">
+        <f t="shared" si="2"/>
+        <v>29.2</v>
+      </c>
+      <c r="P13" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="3">
+        <v>8</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3">
+        <v>16</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="L14" s="35" t="s">
+        <v>319</v>
+      </c>
+      <c r="M14" s="29">
+        <v>50</v>
+      </c>
+      <c r="N14" s="37">
+        <v>2.9100000000000001E-2</v>
+      </c>
+      <c r="O14" s="32">
+        <f t="shared" ref="O14:O15" si="4">M14*N14</f>
+        <v>1.4550000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="3">
+        <v>8</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3">
+        <v>16</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="L15" s="35" t="s">
+        <v>320</v>
+      </c>
+      <c r="M15" s="29">
+        <v>50</v>
+      </c>
+      <c r="N15" s="37">
+        <v>2.75E-2</v>
+      </c>
+      <c r="O15" s="32">
+        <f t="shared" si="4"/>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="3">
+        <v>8</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3">
+        <f>16*3</f>
+        <v>48</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="L16" s="35" t="s">
+        <v>321</v>
+      </c>
+      <c r="M16" s="29">
+        <v>200</v>
+      </c>
+      <c r="N16" s="37">
+        <v>7.8E-2</v>
+      </c>
+      <c r="O16" s="32">
+        <f t="shared" si="1"/>
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="3">
+        <v>9</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L17" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="M17" s="29">
+        <v>50</v>
+      </c>
+      <c r="N17" s="37">
+        <v>4.7E-2</v>
+      </c>
+      <c r="O17" s="32">
+        <f t="shared" si="1"/>
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="L18" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="M18" s="29">
+        <v>20</v>
+      </c>
+      <c r="N18" s="37">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="O18" s="32">
+        <f t="shared" si="1"/>
+        <v>5.1400000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="L19" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="M19" s="29">
+        <v>10</v>
+      </c>
+      <c r="N19" s="37">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="O19" s="32">
+        <f t="shared" si="1"/>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="L20" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="M20" s="29">
+        <v>10</v>
+      </c>
+      <c r="N20" s="37">
+        <v>5.5E-2</v>
+      </c>
+      <c r="O20" s="32">
+        <f t="shared" si="1"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L21" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="M21" s="29">
+        <v>10</v>
+      </c>
+      <c r="N21" s="37">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="O21" s="32">
+        <f t="shared" si="1"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="L22" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="M22" s="29">
+        <v>10</v>
+      </c>
+      <c r="N22" s="37">
+        <v>5.5E-2</v>
+      </c>
+      <c r="O22" s="32">
+        <f t="shared" si="1"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L23" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="M23" s="29">
+        <v>10</v>
+      </c>
+      <c r="N23" s="37">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O23" s="32">
+        <f t="shared" si="1"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="54" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="3">
+        <v>8</v>
+      </c>
+      <c r="H24" s="3">
+        <v>30</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="L24" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="M24" s="29">
+        <v>200</v>
+      </c>
+      <c r="N24" s="37">
+        <v>0.02</v>
+      </c>
+      <c r="O24" s="32">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>3</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="M25" s="29">
+        <v>30</v>
+      </c>
+      <c r="N25" s="37">
+        <v>4.7E-2</v>
+      </c>
+      <c r="O25" s="32">
+        <f t="shared" si="1"/>
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="L26" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="M26" s="29">
+        <v>30</v>
+      </c>
+      <c r="N26" s="37">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O26" s="32">
+        <f t="shared" si="1"/>
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="27"/>
+      <c r="E27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L27" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="M27" s="29">
+        <v>4</v>
+      </c>
+      <c r="N27" s="37">
+        <v>16.25</v>
+      </c>
+      <c r="O27" s="32">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L28" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="M28" s="29">
+        <v>15</v>
+      </c>
+      <c r="N28" s="37">
+        <v>1.37</v>
+      </c>
+      <c r="O28" s="32">
+        <f t="shared" si="1"/>
+        <v>20.55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3">
+        <v>3</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L29" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="M29" s="29">
+        <v>12</v>
+      </c>
+      <c r="N29" s="37">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="O29" s="32">
+        <f t="shared" si="1"/>
+        <v>49.800000000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="3">
+        <v>2</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L30" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="M30" s="29">
+        <v>10</v>
+      </c>
+      <c r="N30" s="37">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="O30" s="32">
+        <f t="shared" si="1"/>
+        <v>2.8100000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="3">
+        <v>8</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="L31" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="M31" s="29">
+        <v>50</v>
+      </c>
+      <c r="N31" s="37">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O31" s="32">
+        <f t="shared" si="1"/>
+        <v>2.9499999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="3">
+        <v>8</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L32" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="M32" s="29">
+        <v>50</v>
+      </c>
+      <c r="N32" s="37">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="O32" s="32">
+        <f t="shared" si="1"/>
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="3">
+        <v>3</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="L33" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="M33" s="29">
+        <v>10</v>
+      </c>
+      <c r="N33" s="37">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="O33" s="32">
+        <f t="shared" si="1"/>
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="39" t="s">
+        <v>323</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>2</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="L34" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="M34" s="29">
+        <v>2</v>
+      </c>
+      <c r="N34" s="37">
+        <v>16.079999999999998</v>
+      </c>
+      <c r="O34" s="32">
+        <f t="shared" ref="O34" si="5">M34*N34</f>
+        <v>32.159999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="L35" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="M35" s="29">
+        <v>2</v>
+      </c>
+      <c r="N35" s="37">
+        <v>11.4</v>
+      </c>
+      <c r="O35" s="32">
+        <f t="shared" si="1"/>
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="3">
+        <v>2</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="L36" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="M36" s="29">
+        <v>10</v>
+      </c>
+      <c r="N36" s="37">
+        <v>3.2280000000000002</v>
+      </c>
+      <c r="O36" s="32">
+        <f t="shared" ref="O36:O37" si="6">M36*N36</f>
+        <v>32.28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="3">
+        <v>2</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="L37" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="M37" s="29">
+        <v>5</v>
+      </c>
+      <c r="N37" s="37">
+        <v>1.6859999999999999</v>
+      </c>
+      <c r="O37" s="32">
+        <f t="shared" si="6"/>
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="2">
+        <v>4</v>
+      </c>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="L38" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="M38" s="29">
+        <v>20</v>
+      </c>
+      <c r="N38" s="37">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="O38" s="32">
+        <f t="shared" si="1"/>
+        <v>6.74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="2">
+        <v>3</v>
+      </c>
+      <c r="H39" s="3">
+        <v>2</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="L39" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="M39" s="29">
+        <v>20</v>
+      </c>
+      <c r="N39" s="37">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="O39" s="32">
+        <f t="shared" ref="O39" si="7">M39*N39</f>
+        <v>4.6999999999999993</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="2">
+        <v>3</v>
+      </c>
+      <c r="H40" s="3">
+        <v>2</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="L40" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="M40" s="29">
+        <v>20</v>
+      </c>
+      <c r="N40" s="37">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="O40" s="32">
+        <f t="shared" si="1"/>
+        <v>8.32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3">
+        <v>36</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="L41" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="M41" s="29">
+        <v>110</v>
+      </c>
+      <c r="N41" s="37">
+        <v>0.106</v>
+      </c>
+      <c r="O41" s="32">
+        <f t="shared" ref="O41" si="8">M41*N41</f>
+        <v>11.66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N42" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="O42" s="34">
+        <f>SUM(O2:O41)</f>
+        <v>568.68000000000006</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L46" s="30" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L47" s="30" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L48" s="30" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="49" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L49" s="30" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="50" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L50" s="30" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="51" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L51" s="30" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="52" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L52" s="30" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="53" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L53" s="30" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O42"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2802,13 +6133,53 @@
         <v>541.4</v>
       </c>
     </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="30" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="30" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="30" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="30" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="30" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="30" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="30" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="30" t="s">
+        <v>313</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
@@ -4181,7 +7552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
@@ -4957,12 +8328,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6841,7 +10212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
@@ -8144,7 +11515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D10"/>
   <sheetViews>

</xml_diff>